<commit_message>
Updated title field  names
</commit_message>
<xml_diff>
--- a/TPS_Report.xlsx
+++ b/TPS_Report.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27430"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16420" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="-20" windowWidth="28800" windowHeight="16420" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,27 +21,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="19">
   <si>
-    <t>task</t>
-  </si>
-  <si>
-    <t>time</t>
-  </si>
-  <si>
-    <t>risk</t>
-  </si>
-  <si>
-    <t>who</t>
-  </si>
-  <si>
-    <t>actual time</t>
-  </si>
-  <si>
-    <t>code complete</t>
-  </si>
-  <si>
-    <t>code review</t>
-  </si>
-  <si>
     <t>Test Doubles</t>
   </si>
   <si>
@@ -63,9 +42,6 @@
     <t>2 hours</t>
   </si>
   <si>
-    <t>Test Inf and -Inf</t>
-  </si>
-  <si>
     <t>45 min</t>
   </si>
   <si>
@@ -76,6 +52,30 @@
   </si>
   <si>
     <t>Skylar</t>
+  </si>
+  <si>
+    <t>Test +Inf and -Inf</t>
+  </si>
+  <si>
+    <t>Assigned</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Task</t>
+  </si>
+  <si>
+    <t>Actual Time</t>
+  </si>
+  <si>
+    <t>Code Complete</t>
+  </si>
+  <si>
+    <t>Reviewer</t>
+  </si>
+  <si>
+    <t>Risk (1-5)</t>
   </si>
 </sst>
 </file>
@@ -466,32 +466,36 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17:D18"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="15" customWidth="1"/>
+    <col min="6" max="6" width="14" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="3" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -505,94 +509,94 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="1" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C3" s="1">
         <v>3</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="F3" s="2">
         <v>1</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="1" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C4" s="1">
         <v>3</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="F4" s="2">
         <v>1</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C5" s="1">
         <v>4</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="F5" s="2">
         <v>1</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C6" s="1">
         <v>2</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="F6" s="2">
         <v>1</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Addition of Absolute Error, and Relative Error spike creations
</commit_message>
<xml_diff>
--- a/TPS_Report.xlsx
+++ b/TPS_Report.xlsx
@@ -507,7 +507,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:G6"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -602,7 +602,7 @@
         <v>11</v>
       </c>
       <c r="F4" s="2">
-        <v>0.25</v>
+        <v>0.05</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>3</v>

</xml_diff>